<commit_message>
ci(bench): fix setup-node cache ordering, add summarize, docs; bench.js --timeout option
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -4,28 +4,96 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Export" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Summary" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="High" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="All" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
   <si>
     <t>domain</t>
   </si>
   <si>
-    <t>status</t>
+    <t>https</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>dns</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>reasonCode</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>openai.com</t>
+  </si>
+  <si>
+    <t>{"ok":false,"status":403,"redirects":0,"finalUrl":"https://openai.com/","elapsedMs":229,"history":[],"tls":{"issuer":"Let's Encrypt","sni":"openai.com"},"errorType":"http4xx"}</t>
+  </si>
+  <si>
+    <t>{"ok":false,"status":403,"redirects":1,"finalUrl":"https://openai.com/","elapsedMs":184,"history":[{"url":"http://openai.com/","status":301}],"errorType":"http4xx"}</t>
+  </si>
+  <si>
+    <t>{"status":"NOERROR","chain":[{"type":"A","data":"172.64.154.211","ttl":10},{"type":"A","data":"104.18.33.45","ttl":10}],"elapsedMs":106,"queries":[{"type":"A","status":"NOERROR","elapsedMs":106,"answers":2}]}</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>HTTP/TLS all failed</t>
+  </si>
+  <si>
+    <t>HTTP_ALL_FAILED</t>
   </si>
   <si>
     <t>example.com</t>
   </si>
   <si>
+    <t>{"ok":true,"status":200,"redirects":0,"finalUrl":"https://example.com/","elapsedMs":1063,"history":[],"tls":{"issuer":"DigiCert Inc","sni":"example.com"}}</t>
+  </si>
+  <si>
+    <t>{"ok":false}</t>
+  </si>
+  <si>
+    <t>{"status":"NOERROR","chain":[{"type":"A","data":"23.215.0.136","ttl":179},{"type":"A","data":"23.192.228.80","ttl":179},{"type":"A","data":"23.215.0.138","ttl":179},{"type":"A","data":"96.7.128.175","ttl":179},{"type":"A","data":"96.7.128.198","ttl":179},{"type":"A","data":"23.192.228.84","ttl":179}],"elapsedMs":134,"queries":[{"type":"A","status":"NOERROR","elapsedMs":134,"answers":6}]}</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
     <t>ok</t>
   </si>
   <si>
-    <t>openai.com</t>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -402,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -417,16 +485,191 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>